<commit_message>
Opdatering af punkterne med Excel arket
</commit_message>
<xml_diff>
--- a/excel/FM.xlsx
+++ b/excel/FM.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="239">
   <si>
     <t>Projekt</t>
   </si>
@@ -100,7 +100,7 @@
     <t>Sigridsvej 46</t>
   </si>
   <si>
-    <t>56.1565956,10.1307686</t>
+    <t>56.156899, 10.135274</t>
   </si>
   <si>
     <t>Brabrand Elektricitetsselskab I/S</t>
@@ -176,6 +176,561 @@
   </si>
   <si>
     <t>56.161213, 10.139823</t>
+  </si>
+  <si>
+    <t>Motel Tre Ege</t>
+  </si>
+  <si>
+    <t>Møllevej 15</t>
+  </si>
+  <si>
+    <t>Erhvervsbyggerier</t>
+  </si>
+  <si>
+    <t>Leo Bødker Nielsen</t>
+  </si>
+  <si>
+    <t>56.154414, 10.086723</t>
+  </si>
+  <si>
+    <t>Huse for .. og ejendomsmægler</t>
+  </si>
+  <si>
+    <t>Røgelvej 1</t>
+  </si>
+  <si>
+    <t>Egon Hansen og Jens Hansen</t>
+  </si>
+  <si>
+    <t>56.152956, 10.127007</t>
+  </si>
+  <si>
+    <t>F.L. Bie Maskinfabrik</t>
+  </si>
+  <si>
+    <t>Holmstrupgårdsvej 1</t>
+  </si>
+  <si>
+    <t>56.164111, 10.119985</t>
+  </si>
+  <si>
+    <t>Brabrandhus</t>
+  </si>
+  <si>
+    <t>Hovedgaden 54</t>
+  </si>
+  <si>
+    <t>Gunnar Frank (?)</t>
+  </si>
+  <si>
+    <t>56.153726, 10.103720</t>
+  </si>
+  <si>
+    <t>Brabrandhus II</t>
+  </si>
+  <si>
+    <t>Hovedgaden 56 - 58</t>
+  </si>
+  <si>
+    <t>56.153523, 10.103490</t>
+  </si>
+  <si>
+    <t>Udvidelse af Grindstedværket</t>
+  </si>
+  <si>
+    <t>Edwin Rahrsvej 34</t>
+  </si>
+  <si>
+    <t>56.162833, 10.131361</t>
+  </si>
+  <si>
+    <t>3 rækkehuse</t>
+  </si>
+  <si>
+    <t>Skovbakkevej 7 C,D og E</t>
+  </si>
+  <si>
+    <t>Boliggrupper</t>
+  </si>
+  <si>
+    <t>56.154972, 10.107953</t>
+  </si>
+  <si>
+    <t>5 rækkehuse</t>
+  </si>
+  <si>
+    <t>Mariedalsvej 10 - 18</t>
+  </si>
+  <si>
+    <t>Hansen og Hjelm</t>
+  </si>
+  <si>
+    <t>56.157553, 10.098949</t>
+  </si>
+  <si>
+    <t>Tyttebærvej 12 - 18</t>
+  </si>
+  <si>
+    <t>56.154846, 10.119433</t>
+  </si>
+  <si>
+    <t>56 etagebiliger (Blok A og B)</t>
+  </si>
+  <si>
+    <t>Hoffmannsvej 2 - 16</t>
+  </si>
+  <si>
+    <t>Rømerhaven A/S</t>
+  </si>
+  <si>
+    <t>56.155194, 10.104276</t>
+  </si>
+  <si>
+    <t>65 etageboliger (Blok C)</t>
+  </si>
+  <si>
+    <t>Hoffmannsvej 18 - 30</t>
+  </si>
+  <si>
+    <t>56.156225, 10.101945</t>
+  </si>
+  <si>
+    <t>2 ens enfamiliehuse</t>
+  </si>
+  <si>
+    <t>Hoffmannsvej 3 - 5</t>
+  </si>
+  <si>
+    <t>56.155689, 10.101559</t>
+  </si>
+  <si>
+    <t>5 + 5 rækkehuse</t>
+  </si>
+  <si>
+    <t>Ligustervej 1 -9 og 2 - 10</t>
+  </si>
+  <si>
+    <t>56.155757, 10.123577</t>
+  </si>
+  <si>
+    <t>Vandværksvej 2 - 10</t>
+  </si>
+  <si>
+    <t>Svend Andresen</t>
+  </si>
+  <si>
+    <t>56.151876, 10.109425</t>
+  </si>
+  <si>
+    <t>Tingstedet 13 klyngehuse</t>
+  </si>
+  <si>
+    <t>Tingstedet 58 - 96</t>
+  </si>
+  <si>
+    <t>Leo Bøker</t>
+  </si>
+  <si>
+    <t>56.151101, 10.085095</t>
+  </si>
+  <si>
+    <t>Tingstedet 3 klyngehuse</t>
+  </si>
+  <si>
+    <t>Tingstedet 64 - 72 og 80</t>
+  </si>
+  <si>
+    <t>Svend Andresen?</t>
+  </si>
+  <si>
+    <t>56.151621, 10.086034</t>
+  </si>
+  <si>
+    <t>5 A-huse</t>
+  </si>
+  <si>
+    <t>Ørvadsvej 5 - 7</t>
+  </si>
+  <si>
+    <t>Gunnar Frank</t>
+  </si>
+  <si>
+    <t>56.149369, 10.087944</t>
+  </si>
+  <si>
+    <t>18 kollegieværelser</t>
+  </si>
+  <si>
+    <t>Skovbakkevej 21</t>
+  </si>
+  <si>
+    <t>56.156341, 10.109404</t>
+  </si>
+  <si>
+    <t>18 gårdhavehuse på Kroghs jorder</t>
+  </si>
+  <si>
+    <t>Egebjergvej 2 - 36</t>
+  </si>
+  <si>
+    <t>56.160430, 10.117075</t>
+  </si>
+  <si>
+    <t>10 gårdhavehuse på Kroghs jorder</t>
+  </si>
+  <si>
+    <t>Egebjergvej 137 - 155</t>
+  </si>
+  <si>
+    <t>56.158506, 10.112904</t>
+  </si>
+  <si>
+    <t>22 gårdhavehuse på Kroghs jorder</t>
+  </si>
+  <si>
+    <t>Egebjergvej 1 - 41A</t>
+  </si>
+  <si>
+    <t>56.160016, 10.116300</t>
+  </si>
+  <si>
+    <t>Plan og retningslinier for bebyggelse</t>
+  </si>
+  <si>
+    <t>Lykkenshøj 6 - 30 og 32 - 68</t>
+  </si>
+  <si>
+    <t>Eget regi</t>
+  </si>
+  <si>
+    <t>56.158064, 10.106942</t>
+  </si>
+  <si>
+    <t>Lykkenshøj 50 og 56 - 62</t>
+  </si>
+  <si>
+    <t>La Kamilius</t>
+  </si>
+  <si>
+    <t>56.159027, 10.108862</t>
+  </si>
+  <si>
+    <t>7 + 6 gårdhavehuse, 5 + 10 terrassehuse</t>
+  </si>
+  <si>
+    <t>Hejrebakken 13 - 57, 2 - 32</t>
+  </si>
+  <si>
+    <t>Boligf.Bikuben</t>
+  </si>
+  <si>
+    <t>56.157348, 10.123950</t>
+  </si>
+  <si>
+    <t>126 etageboliger, Hans Broges Bakker</t>
+  </si>
+  <si>
+    <t>J.P. Larsensvej 112 - 128</t>
+  </si>
+  <si>
+    <t>Kurt Thorsen</t>
+  </si>
+  <si>
+    <t>56.155126, 10.105206</t>
+  </si>
+  <si>
+    <t>9 rækkehusboliger i tre etager</t>
+  </si>
+  <si>
+    <t>Skovbakkevej 9 C - K</t>
+  </si>
+  <si>
+    <t>56.155929, 10.107341</t>
+  </si>
+  <si>
+    <t>4 dobbelthuse, 16 boliger</t>
+  </si>
+  <si>
+    <t>J.P. Larsensvej 23 - 29</t>
+  </si>
+  <si>
+    <t>56.154574, 10.106577</t>
+  </si>
+  <si>
+    <t>Hus for E. Kornerup</t>
+  </si>
+  <si>
+    <t>Hans Brogesvej 33</t>
+  </si>
+  <si>
+    <t>Enfamilieboliger</t>
+  </si>
+  <si>
+    <t>Ernst Kornerup</t>
+  </si>
+  <si>
+    <t>56.156089, 10.117217</t>
+  </si>
+  <si>
+    <t>Hus for tømrermester Møller</t>
+  </si>
+  <si>
+    <t>Silkeborgvej 683</t>
+  </si>
+  <si>
+    <t>Frode Møller</t>
+  </si>
+  <si>
+    <t>56.153034, 10.093043</t>
+  </si>
+  <si>
+    <t>Hus for murermester Hjelm</t>
+  </si>
+  <si>
+    <t>Silkeborgvej 687</t>
+  </si>
+  <si>
+    <t>Harald Hjelm</t>
+  </si>
+  <si>
+    <t>56.153007, 10.092310</t>
+  </si>
+  <si>
+    <t>Hus for speditør Erichsen</t>
+  </si>
+  <si>
+    <t>Søparkvej 7</t>
+  </si>
+  <si>
+    <t>Knud Erichsen</t>
+  </si>
+  <si>
+    <t>56.151766, 10.107274</t>
+  </si>
+  <si>
+    <t>Hus for civ.ing. Sv. Jensen</t>
+  </si>
+  <si>
+    <t>Tyttebærvej 5</t>
+  </si>
+  <si>
+    <t>Svend Jensen</t>
+  </si>
+  <si>
+    <t>56.155215, 10.119814</t>
+  </si>
+  <si>
+    <t>Eget hus, Knud Friis</t>
+  </si>
+  <si>
+    <t>Højen 13</t>
+  </si>
+  <si>
+    <t>Knud Friis</t>
+  </si>
+  <si>
+    <t>56.157269, 10.111467</t>
+  </si>
+  <si>
+    <t>Hus for overlæge Leth-Petersen</t>
+  </si>
+  <si>
+    <t>Højen 6</t>
+  </si>
+  <si>
+    <t>A. Leth-Petersen</t>
+  </si>
+  <si>
+    <t>56.157762, 10.111153</t>
+  </si>
+  <si>
+    <t>Hus for mælkehandler Christiansen</t>
+  </si>
+  <si>
+    <t>J.P.Larsensvej 38A</t>
+  </si>
+  <si>
+    <t>Johs. Christiansen</t>
+  </si>
+  <si>
+    <t>56.155239, 10.112250</t>
+  </si>
+  <si>
+    <t>Hus for driftsbestyrer Larsen</t>
+  </si>
+  <si>
+    <t>Stenbækvej 15</t>
+  </si>
+  <si>
+    <t>Otto Larsen</t>
+  </si>
+  <si>
+    <t>56.155657, 10.117727</t>
+  </si>
+  <si>
+    <t>Hus for manufakturhandler Poulsen</t>
+  </si>
+  <si>
+    <t>Søvej 3A</t>
+  </si>
+  <si>
+    <t>Aage Poulsen</t>
+  </si>
+  <si>
+    <t>56.151997, 10.104694</t>
+  </si>
+  <si>
+    <t>Hus for direktør Dalgaard Sørensen</t>
+  </si>
+  <si>
+    <t>Engdalsvej 18</t>
+  </si>
+  <si>
+    <t>Henry Dalgaard Sørensen</t>
+  </si>
+  <si>
+    <t>56.151834, 10.108527</t>
+  </si>
+  <si>
+    <t>Hus for civ.ing. Bigaard Sørensen</t>
+  </si>
+  <si>
+    <t>Lyngbakkevej 8</t>
+  </si>
+  <si>
+    <t>Bent Bigaard Sørensen</t>
+  </si>
+  <si>
+    <t>56.157341, 10.112349</t>
+  </si>
+  <si>
+    <t>Hus for tandlæge Sørensen</t>
+  </si>
+  <si>
+    <t>Hougårdsvej 31</t>
+  </si>
+  <si>
+    <t>Holger Sørensen</t>
+  </si>
+  <si>
+    <t>56.150674, 10.094461</t>
+  </si>
+  <si>
+    <t>Hus for lærer Dohm</t>
+  </si>
+  <si>
+    <t>Quistgårdsvej 1</t>
+  </si>
+  <si>
+    <t>Bent Dohm</t>
+  </si>
+  <si>
+    <t>56.151833, 10.105354</t>
+  </si>
+  <si>
+    <t>Hus for install.mester Ejstrup</t>
+  </si>
+  <si>
+    <t>Hørstykkevej 3</t>
+  </si>
+  <si>
+    <t>Gunnar Ejstrup</t>
+  </si>
+  <si>
+    <t>56.155250, 10.120688</t>
+  </si>
+  <si>
+    <t>Hus for direktør Johansen</t>
+  </si>
+  <si>
+    <t>Edwin Rahsvej 61</t>
+  </si>
+  <si>
+    <t>Willy "Derby" Johansen</t>
+  </si>
+  <si>
+    <t>56.163032, 10.118521</t>
+  </si>
+  <si>
+    <t>Hus for export manager Godfrey</t>
+  </si>
+  <si>
+    <t>Lyngbakkevej 10</t>
+  </si>
+  <si>
+    <t>A.B. Godfrey</t>
+  </si>
+  <si>
+    <t>56.158149, 10.112746</t>
+  </si>
+  <si>
+    <t>Hus for gartner Harmsen</t>
+  </si>
+  <si>
+    <t>Skibbyvej 11</t>
+  </si>
+  <si>
+    <t>Helge Harmsen</t>
+  </si>
+  <si>
+    <t>56.150390, 10.069753</t>
+  </si>
+  <si>
+    <t>Hus for Revisor Lund</t>
+  </si>
+  <si>
+    <t>Lykkensdalsvej 6C</t>
+  </si>
+  <si>
+    <t>C.Lund</t>
+  </si>
+  <si>
+    <t>56.157142, 10.102784</t>
+  </si>
+  <si>
+    <t>Hus for speciallæge Andersson</t>
+  </si>
+  <si>
+    <t>Hans Brogesvej 3C</t>
+  </si>
+  <si>
+    <t>Poul G. Andersson</t>
+  </si>
+  <si>
+    <t>56.1560404,10.1111153</t>
+  </si>
+  <si>
+    <t>Tilbygning og indvendig indretning</t>
+  </si>
+  <si>
+    <t>Engdalsvej 74 C</t>
+  </si>
+  <si>
+    <t>Mogens Vigh Larsen</t>
+  </si>
+  <si>
+    <t>56.150104, 10.115291</t>
+  </si>
+  <si>
+    <t>Enfamiliehus</t>
+  </si>
+  <si>
+    <t>Lykkenshøj 24</t>
+  </si>
+  <si>
+    <t>56.157350, 10.106086</t>
+  </si>
+  <si>
+    <t>Hus for Jerløv og Troelsen</t>
+  </si>
+  <si>
+    <t>Lyngbakkevej 12</t>
+  </si>
+  <si>
+    <t>Jerløv og Troelsen</t>
+  </si>
+  <si>
+    <t>56.158226, 10.113342</t>
   </si>
 </sst>
 </file>
@@ -183,7 +738,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -200,12 +755,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -314,7 +863,7 @@
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
@@ -946,405 +1495,989 @@
         <v>53</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
-      <c r="A17" s="10"/>
-      <c r="B17" s="10"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="10"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
-      <c r="A18" s="10"/>
-      <c r="B18" s="10"/>
-      <c r="C18" s="11"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
-      <c r="A19" s="10"/>
-      <c r="B19" s="10"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="10"/>
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
+      <c r="A17" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="C17" s="11">
+        <v>1962</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="F17" s="10" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
+      <c r="A18" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="C18" s="11">
+        <v>1963</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="F18" s="10" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
+      <c r="A19" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="C19" s="11">
+        <v>1966</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>56</v>
+      </c>
       <c r="E19" s="10"/>
-      <c r="F19" s="10"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
-      <c r="A20" s="10"/>
-      <c r="B20" s="10"/>
-      <c r="C20" s="11"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="10"/>
+      <c r="F19" s="10" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
+      <c r="A20" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="C20" s="11">
+        <v>1971</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="F20" s="10" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
-      <c r="A21" s="10"/>
-      <c r="B21" s="10"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="10"/>
+      <c r="A21" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="C21" s="12">
+        <v>1987</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>56</v>
+      </c>
       <c r="E21" s="10"/>
-      <c r="F21" s="10"/>
+      <c r="F21" s="10" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
-      <c r="A22" s="10"/>
-      <c r="B22" s="10"/>
-      <c r="C22" s="12"/>
-      <c r="D22" s="10"/>
+      <c r="A22" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="C22" s="12">
+        <v>1990</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>56</v>
+      </c>
       <c r="E22" s="10"/>
-      <c r="F22" s="10"/>
+      <c r="F22" s="10" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
-      <c r="A23" s="10"/>
-      <c r="B23" s="10"/>
-      <c r="C23" s="12"/>
-      <c r="D23" s="10"/>
+      <c r="A23" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="C23" s="12">
+        <v>1955</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>78</v>
+      </c>
       <c r="E23" s="10"/>
-      <c r="F23" s="10"/>
+      <c r="F23" s="10" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
-      <c r="A24" s="10"/>
-      <c r="B24" s="10"/>
-      <c r="C24" s="12"/>
-      <c r="D24" s="10"/>
-      <c r="E24" s="10"/>
-      <c r="F24" s="10"/>
+      <c r="A24" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="C24" s="12">
+        <v>1956</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="E24" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="F24" s="10" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
-      <c r="A25" s="10"/>
-      <c r="B25" s="10"/>
-      <c r="C25" s="12"/>
-      <c r="D25" s="10"/>
-      <c r="E25" s="10"/>
-      <c r="F25" s="10"/>
+      <c r="A25" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="C25" s="12">
+        <v>1960</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="E25" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="F25" s="10" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
-      <c r="A26" s="10"/>
-      <c r="B26" s="10"/>
-      <c r="C26" s="12"/>
-      <c r="D26" s="10"/>
-      <c r="E26" s="10"/>
-      <c r="F26" s="10"/>
+      <c r="A26" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="C26" s="12">
+        <v>1963</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="E26" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="F26" s="10" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
-      <c r="A27" s="10"/>
-      <c r="B27" s="10"/>
-      <c r="C27" s="12"/>
-      <c r="D27" s="10"/>
-      <c r="E27" s="10"/>
-      <c r="F27" s="10"/>
+      <c r="A27" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="C27" s="12">
+        <v>1966</v>
+      </c>
+      <c r="D27" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="E27" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="F27" s="10" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
-      <c r="A28" s="10"/>
-      <c r="B28" s="10"/>
-      <c r="C28" s="12"/>
-      <c r="D28" s="10"/>
-      <c r="E28" s="10"/>
-      <c r="F28" s="10"/>
+      <c r="A28" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="B28" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="C28" s="12">
+        <v>1967</v>
+      </c>
+      <c r="D28" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="E28" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="F28" s="10" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
-      <c r="A29" s="10"/>
-      <c r="B29" s="10"/>
-      <c r="C29" s="12"/>
-      <c r="D29" s="10"/>
-      <c r="E29" s="10"/>
-      <c r="F29" s="10"/>
+      <c r="A29" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="B29" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="C29" s="12">
+        <v>1966</v>
+      </c>
+      <c r="D29" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="E29" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="F29" s="10" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
-      <c r="A30" s="10"/>
-      <c r="B30" s="10"/>
-      <c r="C30" s="12"/>
-      <c r="D30" s="10"/>
-      <c r="E30" s="10"/>
-      <c r="F30" s="10"/>
+      <c r="A30" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B30" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="C30" s="12">
+        <v>1965</v>
+      </c>
+      <c r="D30" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="E30" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="F30" s="10" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
-      <c r="A31" s="10"/>
-      <c r="B31" s="10"/>
-      <c r="C31" s="12"/>
-      <c r="D31" s="10"/>
-      <c r="E31" s="10"/>
-      <c r="F31" s="10"/>
+      <c r="A31" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="B31" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="C31" s="12">
+        <v>1967</v>
+      </c>
+      <c r="D31" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="E31" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="F31" s="10" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75">
-      <c r="A32" s="10"/>
-      <c r="B32" s="10"/>
-      <c r="C32" s="12"/>
-      <c r="D32" s="10"/>
-      <c r="E32" s="10"/>
-      <c r="F32" s="10"/>
+      <c r="A32" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="B32" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="C32" s="12">
+        <v>1967</v>
+      </c>
+      <c r="D32" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="E32" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="F32" s="10" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75">
-      <c r="A33" s="10"/>
-      <c r="B33" s="10"/>
-      <c r="C33" s="12"/>
-      <c r="D33" s="10"/>
-      <c r="E33" s="10"/>
-      <c r="F33" s="10"/>
+      <c r="A33" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="B33" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="C33" s="12">
+        <v>1968</v>
+      </c>
+      <c r="D33" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="E33" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="F33" s="10" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75">
-      <c r="A34" s="10"/>
-      <c r="B34" s="10"/>
-      <c r="C34" s="12"/>
-      <c r="D34" s="10"/>
+      <c r="A34" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="B34" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="C34" s="12">
+        <v>1968</v>
+      </c>
+      <c r="D34" s="10" t="s">
+        <v>78</v>
+      </c>
       <c r="E34" s="10"/>
-      <c r="F34" s="10"/>
+      <c r="F34" s="10" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18.75">
-      <c r="A35" s="10"/>
-      <c r="B35" s="10"/>
-      <c r="C35" s="12"/>
-      <c r="D35" s="10"/>
-      <c r="E35" s="10"/>
-      <c r="F35" s="10"/>
+      <c r="A35" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="B35" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="C35" s="12">
+        <v>1971</v>
+      </c>
+      <c r="D35" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="E35" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="F35" s="10" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18.75">
-      <c r="A36" s="10"/>
-      <c r="B36" s="10"/>
-      <c r="C36" s="12"/>
-      <c r="D36" s="10"/>
-      <c r="E36" s="10"/>
-      <c r="F36" s="10"/>
+      <c r="A36" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="B36" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="C36" s="12">
+        <v>1972</v>
+      </c>
+      <c r="D36" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="E36" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="F36" s="10" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="18.75">
-      <c r="A37" s="10"/>
-      <c r="B37" s="10"/>
-      <c r="C37" s="12"/>
-      <c r="D37" s="10"/>
-      <c r="E37" s="10"/>
-      <c r="F37" s="10"/>
+      <c r="A37" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="B37" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="C37" s="12">
+        <v>1974</v>
+      </c>
+      <c r="D37" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="E37" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="F37" s="10" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="18.75">
-      <c r="A38" s="10"/>
-      <c r="B38" s="10"/>
-      <c r="C38" s="12"/>
-      <c r="D38" s="10"/>
-      <c r="E38" s="10"/>
-      <c r="F38" s="10"/>
+      <c r="A38" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="B38" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="C38" s="12">
+        <v>1973</v>
+      </c>
+      <c r="D38" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="E38" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="F38" s="10" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="18.75">
-      <c r="A39" s="10"/>
-      <c r="B39" s="10"/>
-      <c r="C39" s="12"/>
-      <c r="D39" s="10"/>
-      <c r="E39" s="10"/>
-      <c r="F39" s="10"/>
+      <c r="A39" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B39" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="C39" s="12">
+        <v>1978</v>
+      </c>
+      <c r="D39" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="E39" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="F39" s="10" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="18.75">
-      <c r="A40" s="10"/>
-      <c r="B40" s="10"/>
-      <c r="C40" s="12"/>
-      <c r="D40" s="10"/>
-      <c r="E40" s="10"/>
-      <c r="F40" s="10"/>
+      <c r="A40" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="B40" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="C40" s="12">
+        <v>1977</v>
+      </c>
+      <c r="D40" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="E40" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="F40" s="10" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="18.75">
-      <c r="A41" s="10"/>
-      <c r="B41" s="10"/>
-      <c r="C41" s="12"/>
-      <c r="D41" s="10"/>
-      <c r="E41" s="10"/>
-      <c r="F41" s="10"/>
+      <c r="A41" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="B41" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="C41" s="12">
+        <v>1991</v>
+      </c>
+      <c r="D41" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="E41" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="F41" s="10" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="18.75">
-      <c r="A42" s="10"/>
-      <c r="B42" s="10"/>
-      <c r="C42" s="12"/>
-      <c r="D42" s="10"/>
+      <c r="A42" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="B42" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="C42" s="12">
+        <v>2005</v>
+      </c>
+      <c r="D42" s="10" t="s">
+        <v>78</v>
+      </c>
       <c r="E42" s="10"/>
-      <c r="F42" s="10"/>
+      <c r="F42" s="10" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="18.75">
-      <c r="A43" s="10"/>
-      <c r="B43" s="10"/>
-      <c r="C43" s="12"/>
-      <c r="D43" s="10"/>
+      <c r="A43" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="B43" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="C43" s="12">
+        <v>2006</v>
+      </c>
+      <c r="D43" s="10" t="s">
+        <v>78</v>
+      </c>
       <c r="E43" s="10"/>
-      <c r="F43" s="10"/>
+      <c r="F43" s="10" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="18.75">
-      <c r="A44" s="10"/>
-      <c r="B44" s="10"/>
-      <c r="C44" s="12"/>
-      <c r="D44" s="10"/>
-      <c r="E44" s="10"/>
-      <c r="F44" s="10"/>
+      <c r="A44" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="B44" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="C44" s="12">
+        <v>1952</v>
+      </c>
+      <c r="D44" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="E44" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="F44" s="10" t="s">
+        <v>151</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="18.75">
-      <c r="A45" s="10"/>
-      <c r="B45" s="10"/>
-      <c r="C45" s="12"/>
-      <c r="D45" s="10"/>
-      <c r="E45" s="10"/>
-      <c r="F45" s="10"/>
+      <c r="A45" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="B45" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="C45" s="12">
+        <v>1953</v>
+      </c>
+      <c r="D45" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="E45" s="10" t="s">
+        <v>154</v>
+      </c>
+      <c r="F45" s="10" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="18.75">
-      <c r="A46" s="10"/>
-      <c r="B46" s="10"/>
-      <c r="C46" s="12"/>
-      <c r="D46" s="10"/>
-      <c r="E46" s="10"/>
-      <c r="F46" s="10"/>
+      <c r="A46" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="B46" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="C46" s="12">
+        <v>1955</v>
+      </c>
+      <c r="D46" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="E46" s="10" t="s">
+        <v>158</v>
+      </c>
+      <c r="F46" s="10" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="18.75">
-      <c r="A47" s="10"/>
-      <c r="B47" s="10"/>
-      <c r="C47" s="12"/>
-      <c r="D47" s="10"/>
-      <c r="E47" s="10"/>
-      <c r="F47" s="10"/>
+      <c r="A47" s="10" t="s">
+        <v>160</v>
+      </c>
+      <c r="B47" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="C47" s="12">
+        <v>1956</v>
+      </c>
+      <c r="D47" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="E47" s="10" t="s">
+        <v>162</v>
+      </c>
+      <c r="F47" s="10" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="18.75">
-      <c r="A48" s="10"/>
-      <c r="B48" s="10"/>
-      <c r="C48" s="12"/>
-      <c r="D48" s="10"/>
-      <c r="E48" s="10"/>
-      <c r="F48" s="10"/>
+      <c r="A48" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="B48" s="10" t="s">
+        <v>165</v>
+      </c>
+      <c r="C48" s="12">
+        <v>1958</v>
+      </c>
+      <c r="D48" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="E48" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="F48" s="10" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="18.75">
-      <c r="A49" s="10"/>
-      <c r="B49" s="10"/>
-      <c r="C49" s="12"/>
-      <c r="D49" s="10"/>
-      <c r="E49" s="10"/>
-      <c r="F49" s="10"/>
+      <c r="A49" s="10" t="s">
+        <v>168</v>
+      </c>
+      <c r="B49" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="C49" s="12">
+        <v>1958</v>
+      </c>
+      <c r="D49" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="E49" s="10" t="s">
+        <v>170</v>
+      </c>
+      <c r="F49" s="10" t="s">
+        <v>171</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="18.75">
-      <c r="A50" s="10"/>
-      <c r="B50" s="10"/>
-      <c r="C50" s="12"/>
-      <c r="D50" s="10"/>
-      <c r="E50" s="10"/>
-      <c r="F50" s="10"/>
+      <c r="A50" s="10" t="s">
+        <v>172</v>
+      </c>
+      <c r="B50" s="10" t="s">
+        <v>173</v>
+      </c>
+      <c r="C50" s="12">
+        <v>1960</v>
+      </c>
+      <c r="D50" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="E50" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="F50" s="10" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="18.75">
-      <c r="A51" s="10"/>
-      <c r="B51" s="10"/>
-      <c r="C51" s="12"/>
-      <c r="D51" s="10"/>
-      <c r="E51" s="10"/>
-      <c r="F51" s="10"/>
+      <c r="A51" s="10" t="s">
+        <v>176</v>
+      </c>
+      <c r="B51" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="C51" s="12">
+        <v>1961</v>
+      </c>
+      <c r="D51" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="E51" s="10" t="s">
+        <v>178</v>
+      </c>
+      <c r="F51" s="10" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="18.75">
-      <c r="A52" s="10"/>
-      <c r="B52" s="10"/>
-      <c r="C52" s="12"/>
-      <c r="D52" s="10"/>
-      <c r="E52" s="10"/>
-      <c r="F52" s="10"/>
+      <c r="A52" s="10" t="s">
+        <v>180</v>
+      </c>
+      <c r="B52" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="C52" s="12">
+        <v>1960</v>
+      </c>
+      <c r="D52" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="E52" s="10" t="s">
+        <v>182</v>
+      </c>
+      <c r="F52" s="10" t="s">
+        <v>183</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="18.75">
-      <c r="A53" s="10"/>
-      <c r="B53" s="10"/>
-      <c r="C53" s="12"/>
-      <c r="D53" s="10"/>
-      <c r="E53" s="10"/>
-      <c r="F53" s="10"/>
+      <c r="A53" s="10" t="s">
+        <v>184</v>
+      </c>
+      <c r="B53" s="10" t="s">
+        <v>185</v>
+      </c>
+      <c r="C53" s="12">
+        <v>1961</v>
+      </c>
+      <c r="D53" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="E53" s="10" t="s">
+        <v>186</v>
+      </c>
+      <c r="F53" s="10" t="s">
+        <v>187</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="18.75">
-      <c r="A54" s="10"/>
-      <c r="B54" s="10"/>
-      <c r="C54" s="12"/>
-      <c r="D54" s="10"/>
-      <c r="E54" s="10"/>
-      <c r="F54" s="10"/>
+      <c r="A54" s="10" t="s">
+        <v>188</v>
+      </c>
+      <c r="B54" s="10" t="s">
+        <v>189</v>
+      </c>
+      <c r="C54" s="12">
+        <v>1961</v>
+      </c>
+      <c r="D54" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="E54" s="10" t="s">
+        <v>190</v>
+      </c>
+      <c r="F54" s="10" t="s">
+        <v>191</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="18.75">
-      <c r="A55" s="10"/>
-      <c r="B55" s="10"/>
-      <c r="C55" s="12"/>
-      <c r="D55" s="10"/>
-      <c r="E55" s="10"/>
-      <c r="F55" s="10"/>
+      <c r="A55" s="10" t="s">
+        <v>192</v>
+      </c>
+      <c r="B55" s="10" t="s">
+        <v>193</v>
+      </c>
+      <c r="C55" s="12">
+        <v>1961</v>
+      </c>
+      <c r="D55" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="E55" s="10" t="s">
+        <v>194</v>
+      </c>
+      <c r="F55" s="10" t="s">
+        <v>195</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="18.75">
-      <c r="A56" s="10"/>
-      <c r="B56" s="10"/>
-      <c r="C56" s="12"/>
-      <c r="D56" s="10"/>
-      <c r="E56" s="10"/>
-      <c r="F56" s="10"/>
+      <c r="A56" s="10" t="s">
+        <v>196</v>
+      </c>
+      <c r="B56" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="C56" s="12">
+        <v>1962</v>
+      </c>
+      <c r="D56" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="E56" s="10" t="s">
+        <v>198</v>
+      </c>
+      <c r="F56" s="10" t="s">
+        <v>199</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="18.75">
-      <c r="A57" s="10"/>
-      <c r="B57" s="10"/>
-      <c r="C57" s="12"/>
-      <c r="D57" s="10"/>
-      <c r="E57" s="10"/>
-      <c r="F57" s="10"/>
+      <c r="A57" s="10" t="s">
+        <v>200</v>
+      </c>
+      <c r="B57" s="10" t="s">
+        <v>201</v>
+      </c>
+      <c r="C57" s="12">
+        <v>1962</v>
+      </c>
+      <c r="D57" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="E57" s="10" t="s">
+        <v>202</v>
+      </c>
+      <c r="F57" s="10" t="s">
+        <v>203</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="18.75">
-      <c r="A58" s="10"/>
-      <c r="B58" s="10"/>
-      <c r="C58" s="12"/>
-      <c r="D58" s="10"/>
-      <c r="E58" s="10"/>
-      <c r="F58" s="10"/>
+      <c r="A58" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="B58" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="C58" s="12">
+        <v>1963</v>
+      </c>
+      <c r="D58" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="E58" s="10" t="s">
+        <v>206</v>
+      </c>
+      <c r="F58" s="10" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="18.75">
-      <c r="A59" s="10"/>
-      <c r="B59" s="10"/>
-      <c r="C59" s="12"/>
-      <c r="D59" s="10"/>
-      <c r="E59" s="10"/>
-      <c r="F59" s="10"/>
+      <c r="A59" s="10" t="s">
+        <v>208</v>
+      </c>
+      <c r="B59" s="10" t="s">
+        <v>209</v>
+      </c>
+      <c r="C59" s="12">
+        <v>1963</v>
+      </c>
+      <c r="D59" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="E59" s="10" t="s">
+        <v>210</v>
+      </c>
+      <c r="F59" s="10" t="s">
+        <v>211</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="18.75">
-      <c r="A60" s="10"/>
-      <c r="B60" s="10"/>
-      <c r="C60" s="12"/>
-      <c r="D60" s="10"/>
-      <c r="E60" s="10"/>
-      <c r="F60" s="10"/>
+      <c r="A60" s="10" t="s">
+        <v>212</v>
+      </c>
+      <c r="B60" s="10" t="s">
+        <v>213</v>
+      </c>
+      <c r="C60" s="12">
+        <v>1963</v>
+      </c>
+      <c r="D60" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="E60" s="10" t="s">
+        <v>214</v>
+      </c>
+      <c r="F60" s="10" t="s">
+        <v>215</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="18.75">
-      <c r="A61" s="10"/>
-      <c r="B61" s="10"/>
-      <c r="C61" s="12"/>
-      <c r="D61" s="10"/>
-      <c r="E61" s="10"/>
-      <c r="F61" s="10"/>
+      <c r="A61" s="10" t="s">
+        <v>216</v>
+      </c>
+      <c r="B61" s="10" t="s">
+        <v>217</v>
+      </c>
+      <c r="C61" s="12">
+        <v>1965</v>
+      </c>
+      <c r="D61" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="E61" s="10" t="s">
+        <v>218</v>
+      </c>
+      <c r="F61" s="10" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="18.75">
-      <c r="A62" s="10"/>
-      <c r="B62" s="10"/>
-      <c r="C62" s="12"/>
-      <c r="D62" s="10"/>
-      <c r="E62" s="10"/>
-      <c r="F62" s="10"/>
+      <c r="A62" s="10" t="s">
+        <v>220</v>
+      </c>
+      <c r="B62" s="10" t="s">
+        <v>221</v>
+      </c>
+      <c r="C62" s="12">
+        <v>1968</v>
+      </c>
+      <c r="D62" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="E62" s="10" t="s">
+        <v>222</v>
+      </c>
+      <c r="F62" s="10" t="s">
+        <v>223</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="18.75">
-      <c r="A63" s="10"/>
-      <c r="B63" s="10"/>
-      <c r="C63" s="12"/>
-      <c r="D63" s="10"/>
-      <c r="E63" s="10"/>
-      <c r="F63" s="10"/>
+      <c r="A63" s="10" t="s">
+        <v>224</v>
+      </c>
+      <c r="B63" s="10" t="s">
+        <v>225</v>
+      </c>
+      <c r="C63" s="12">
+        <v>1969</v>
+      </c>
+      <c r="D63" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="E63" s="10" t="s">
+        <v>226</v>
+      </c>
+      <c r="F63" s="10" t="s">
+        <v>227</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="18.75">
-      <c r="A64" s="10"/>
-      <c r="B64" s="10"/>
-      <c r="C64" s="12"/>
-      <c r="D64" s="10"/>
-      <c r="E64" s="10"/>
-      <c r="F64" s="10"/>
+      <c r="A64" s="10" t="s">
+        <v>228</v>
+      </c>
+      <c r="B64" s="10" t="s">
+        <v>229</v>
+      </c>
+      <c r="C64" s="12">
+        <v>1974</v>
+      </c>
+      <c r="D64" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="E64" s="10" t="s">
+        <v>230</v>
+      </c>
+      <c r="F64" s="10" t="s">
+        <v>231</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="18.75">
-      <c r="A65" s="10"/>
-      <c r="B65" s="10"/>
-      <c r="C65" s="12"/>
-      <c r="D65" s="10"/>
+      <c r="A65" s="10" t="s">
+        <v>232</v>
+      </c>
+      <c r="B65" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="C65" s="12">
+        <v>1985</v>
+      </c>
+      <c r="D65" s="10" t="s">
+        <v>149</v>
+      </c>
       <c r="E65" s="10"/>
-      <c r="F65" s="10"/>
+      <c r="F65" s="10" t="s">
+        <v>234</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="18.75">
-      <c r="A66" s="10"/>
-      <c r="B66" s="10"/>
-      <c r="C66" s="12"/>
-      <c r="D66" s="10"/>
-      <c r="E66" s="10"/>
-      <c r="F66" s="10"/>
+      <c r="A66" s="10" t="s">
+        <v>235</v>
+      </c>
+      <c r="B66" s="10" t="s">
+        <v>236</v>
+      </c>
+      <c r="C66" s="12">
+        <v>1999</v>
+      </c>
+      <c r="D66" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="E66" s="10" t="s">
+        <v>237</v>
+      </c>
+      <c r="F66" s="10" t="s">
+        <v>238</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="67" customHeight="1" ht="18.75">
       <c r="A67" s="10"/>

</xml_diff>

<commit_message>
opdatering af koordinater i FM.xlsx
</commit_message>
<xml_diff>
--- a/excel/FM.xlsx
+++ b/excel/FM.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="252">
   <si>
     <t>Projekt</t>
   </si>
@@ -43,27 +43,30 @@
     <t>Offentlige bygninger</t>
   </si>
   <si>
+    <t>Sammen med KBP+E43</t>
+  </si>
+  <si>
+    <t>56.153179, 10.119894</t>
+  </si>
+  <si>
+    <t>Brabrand Sygekasse</t>
+  </si>
+  <si>
+    <t>Engdalsvej 6</t>
+  </si>
+  <si>
+    <t>56.152181, 10.103970</t>
+  </si>
+  <si>
+    <t>Gjellerupskolen (/Sødalskolen)</t>
+  </si>
+  <si>
+    <t>Louisevej 29</t>
+  </si>
+  <si>
     <t>Sammen med KBP</t>
   </si>
   <si>
-    <t>56.153179, 10.119894</t>
-  </si>
-  <si>
-    <t>Brabrand Sygekasse</t>
-  </si>
-  <si>
-    <t>Engdalsvej 6</t>
-  </si>
-  <si>
-    <t>56.152181, 10.103970</t>
-  </si>
-  <si>
-    <t>Gjellerupskolen (/Sødalskolen)</t>
-  </si>
-  <si>
-    <t>Louisevej 29</t>
-  </si>
-  <si>
     <t>56.149681, 10.138428</t>
   </si>
   <si>
@@ -91,6 +94,9 @@
     <t>Holmstrupgårdsvej 39</t>
   </si>
   <si>
+    <t>(Dir.f. B&amp;Uforsorg)</t>
+  </si>
+  <si>
     <t>56.174504, 10.117917</t>
   </si>
   <si>
@@ -127,6 +133,9 @@
     <t>Spobjergvej 6</t>
   </si>
   <si>
+    <t>Sammen med KBP o</t>
+  </si>
+  <si>
     <t>56.168670, 10.116093</t>
   </si>
   <si>
@@ -154,7 +163,7 @@
     <t>Engdalsvej 2</t>
   </si>
   <si>
-    <t>(1974 nedrevet)</t>
+    <t>Kontor fra 1974 nedrevet 2009</t>
   </si>
   <si>
     <t>56.151911, 10.101433</t>
@@ -211,6 +220,9 @@
     <t>Holmstrupgårdsvej 1</t>
   </si>
   <si>
+    <t>Virksomheden</t>
+  </si>
+  <si>
     <t>56.164111, 10.119985</t>
   </si>
   <si>
@@ -220,7 +232,7 @@
     <t>Hovedgaden 54</t>
   </si>
   <si>
-    <t>Gunnar Frank (?)</t>
+    <t>B.hus v/ boghdl. K.Marnow</t>
   </si>
   <si>
     <t>56.153726, 10.103720</t>
@@ -232,6 +244,9 @@
     <t>Hovedgaden 56 - 58</t>
   </si>
   <si>
+    <t>Det alm. Danske ejd.selskab A/S</t>
+  </si>
+  <si>
     <t>56.153523, 10.103490</t>
   </si>
   <si>
@@ -241,6 +256,9 @@
     <t>Edwin Rahrsvej 34</t>
   </si>
   <si>
+    <t>Grindsted Products A/S</t>
+  </si>
+  <si>
     <t>56.162833, 10.131361</t>
   </si>
   <si>
@@ -253,6 +271,9 @@
     <t>Boliggrupper</t>
   </si>
   <si>
+    <t>H.Brund, T.Pedersen og J.C.Astrup</t>
+  </si>
+  <si>
     <t>56.154972, 10.107953</t>
   </si>
   <si>
@@ -262,7 +283,7 @@
     <t>Mariedalsvej 10 - 18</t>
   </si>
   <si>
-    <t>Hansen og Hjelm</t>
+    <t>Murermestrene Hansen og H.Hjelm</t>
   </si>
   <si>
     <t>56.157553, 10.098949</t>
@@ -316,9 +337,6 @@
     <t>Vandværksvej 2 - 10</t>
   </si>
   <si>
-    <t>Svend Andresen</t>
-  </si>
-  <si>
     <t>56.151876, 10.109425</t>
   </si>
   <si>
@@ -328,7 +346,7 @@
     <t>Tingstedet 58 - 96</t>
   </si>
   <si>
-    <t>Leo Bøker</t>
+    <t>Svend Andresen (Højbjerg)</t>
   </si>
   <si>
     <t>56.151101, 10.085095</t>
@@ -340,7 +358,7 @@
     <t>Tingstedet 64 - 72 og 80</t>
   </si>
   <si>
-    <t>Svend Andresen?</t>
+    <t>Leo Bødker Nielsen m.fl.</t>
   </si>
   <si>
     <t>56.151621, 10.086034</t>
@@ -352,18 +370,18 @@
     <t>Ørvadsvej 5 - 7</t>
   </si>
   <si>
+    <t>56.149369, 10.087944</t>
+  </si>
+  <si>
+    <t>18 kollegieværelser</t>
+  </si>
+  <si>
+    <t>Skovbakkevej 21</t>
+  </si>
+  <si>
     <t>Gunnar Frank</t>
   </si>
   <si>
-    <t>56.149369, 10.087944</t>
-  </si>
-  <si>
-    <t>18 kollegieværelser</t>
-  </si>
-  <si>
-    <t>Skovbakkevej 21</t>
-  </si>
-  <si>
     <t>56.156341, 10.109404</t>
   </si>
   <si>
@@ -373,6 +391,9 @@
     <t>Egebjergvej 2 - 36</t>
   </si>
   <si>
+    <t>Murermester Erling Nielsen</t>
+  </si>
+  <si>
     <t>56.160430, 10.117075</t>
   </si>
   <si>
@@ -400,51 +421,51 @@
     <t>Lykkenshøj 6 - 30 og 32 - 68</t>
   </si>
   <si>
+    <t>56.158064, 10.106942</t>
+  </si>
+  <si>
+    <t>Lykkenshøj 50 og 56 - 62</t>
+  </si>
+  <si>
     <t>Eget regi</t>
   </si>
   <si>
-    <t>56.158064, 10.106942</t>
-  </si>
-  <si>
-    <t>Lykkenshøj 50 og 56 - 62</t>
+    <t>56.159027, 10.108862</t>
+  </si>
+  <si>
+    <t>7 + 6 gårdhavehuse, 5 + 10 terrassehuse</t>
+  </si>
+  <si>
+    <t>Hejrebakken 13 - 57, 2 - 32</t>
   </si>
   <si>
     <t>La Kamilius</t>
   </si>
   <si>
-    <t>56.159027, 10.108862</t>
-  </si>
-  <si>
-    <t>7 + 6 gårdhavehuse, 5 + 10 terrassehuse</t>
-  </si>
-  <si>
-    <t>Hejrebakken 13 - 57, 2 - 32</t>
+    <t>56.157348, 10.123950</t>
+  </si>
+  <si>
+    <t>126 etageboliger, Hans Broges Bakker</t>
+  </si>
+  <si>
+    <t>J.P. Larsensvej 112 - 128</t>
   </si>
   <si>
     <t>Boligf.Bikuben</t>
   </si>
   <si>
-    <t>56.157348, 10.123950</t>
-  </si>
-  <si>
-    <t>126 etageboliger, Hans Broges Bakker</t>
-  </si>
-  <si>
-    <t>J.P. Larsensvej 112 - 128</t>
+    <t>56.155126, 10.105206</t>
+  </si>
+  <si>
+    <t>9 rækkehusboliger i tre etager</t>
+  </si>
+  <si>
+    <t>Skovbakkevej 9 C - K</t>
   </si>
   <si>
     <t>Kurt Thorsen</t>
   </si>
   <si>
-    <t>56.155126, 10.105206</t>
-  </si>
-  <si>
-    <t>9 rækkehusboliger i tre etager</t>
-  </si>
-  <si>
-    <t>Skovbakkevej 9 C - K</t>
-  </si>
-  <si>
     <t>56.155929, 10.107341</t>
   </si>
   <si>
@@ -454,6 +475,9 @@
     <t>J.P. Larsensvej 23 - 29</t>
   </si>
   <si>
+    <t>Ole Carstensen (?)</t>
+  </si>
+  <si>
     <t>56.154574, 10.106577</t>
   </si>
   <si>
@@ -664,6 +688,18 @@
     <t>56.158149, 10.112746</t>
   </si>
   <si>
+    <t>Hus for Dalsø Flaskegas Compagni</t>
+  </si>
+  <si>
+    <t>Hoffmannsvej 7</t>
+  </si>
+  <si>
+    <t>DFC / Bjørnkjær Savværk</t>
+  </si>
+  <si>
+    <t>56.156023, 10.101376</t>
+  </si>
+  <si>
     <t>Hus for gartner Harmsen</t>
   </si>
   <si>
@@ -716,6 +752,9 @@
   </si>
   <si>
     <t>Lykkenshøj 24</t>
+  </si>
+  <si>
+    <t>H.J.Christiansen, senere E. Dybvad</t>
   </si>
   <si>
     <t>56.157350, 10.106086</t>
@@ -1263,18 +1302,18 @@
         <v>8</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C5" s="8">
         <v>1968</v>
@@ -1283,18 +1322,18 @@
         <v>8</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C6" s="8">
         <v>1968</v>
@@ -1303,18 +1342,18 @@
         <v>8</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C7" s="8">
         <v>1969</v>
@@ -1322,17 +1361,19 @@
       <c r="D7" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="9"/>
+      <c r="E7" s="9" t="s">
+        <v>26</v>
+      </c>
       <c r="F7" s="9" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="7" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C8" s="8">
         <v>1970</v>
@@ -1341,18 +1382,18 @@
         <v>8</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="7" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C9" s="8">
         <v>1971</v>
@@ -1360,17 +1401,19 @@
       <c r="D9" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="9"/>
+      <c r="E9" s="9" t="s">
+        <v>31</v>
+      </c>
       <c r="F9" s="9" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C10" s="8">
         <v>1973</v>
@@ -1380,15 +1423,15 @@
       </c>
       <c r="E10" s="9"/>
       <c r="F10" s="9" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="7" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C11" s="8">
         <v>1973</v>
@@ -1397,18 +1440,18 @@
         <v>8</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>9</v>
+        <v>39</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="7" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C12" s="8">
         <v>1978</v>
@@ -1418,15 +1461,15 @@
       </c>
       <c r="E12" s="9"/>
       <c r="F12" s="9" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="7" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C13" s="8">
         <v>1984</v>
@@ -1436,15 +1479,15 @@
       </c>
       <c r="E13" s="9"/>
       <c r="F13" s="9" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="7" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C14" s="8">
         <v>1982</v>
@@ -1453,18 +1496,18 @@
         <v>8</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
       <c r="A15" s="7" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="C15" s="8">
         <v>1992</v>
@@ -1474,15 +1517,15 @@
       </c>
       <c r="E15" s="9"/>
       <c r="F15" s="9" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
+        <v>53</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="20.25">
       <c r="A16" s="7" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C16" s="8">
         <v>1992</v>
@@ -1492,1000 +1535,1028 @@
       </c>
       <c r="E16" s="9"/>
       <c r="F16" s="9" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
       <c r="A17" s="10" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="C17" s="11">
         <v>1962</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="F17" s="10" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
       <c r="A18" s="10" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="C18" s="11">
         <v>1963</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="F18" s="10" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
       <c r="A19" s="10" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="C19" s="11">
         <v>1966</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="E19" s="10"/>
+        <v>59</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>68</v>
+      </c>
       <c r="F19" s="10" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
       <c r="A20" s="10" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C20" s="11">
         <v>1971</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="F20" s="10" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
       <c r="A21" s="10" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="C21" s="12">
         <v>1987</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="E21" s="10"/>
+        <v>59</v>
+      </c>
+      <c r="E21" s="10" t="s">
+        <v>76</v>
+      </c>
       <c r="F21" s="10" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
       <c r="A22" s="10" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="C22" s="12">
         <v>1990</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="E22" s="10"/>
+        <v>59</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>80</v>
+      </c>
       <c r="F22" s="10" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
       <c r="A23" s="10" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="C23" s="12">
         <v>1955</v>
       </c>
       <c r="D23" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="E23" s="10"/>
+        <v>84</v>
+      </c>
+      <c r="E23" s="10" t="s">
+        <v>85</v>
+      </c>
       <c r="F23" s="10" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
       <c r="A24" s="10" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="C24" s="12">
         <v>1956</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="F24" s="10" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
       <c r="A25" s="10" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="C25" s="12">
         <v>1960</v>
       </c>
       <c r="D25" s="10" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="E25" s="10" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="F25" s="10" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
       <c r="A26" s="10" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="C26" s="12">
         <v>1963</v>
       </c>
       <c r="D26" s="10" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="E26" s="10" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="F26" s="10" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
       <c r="A27" s="10" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>91</v>
+        <v>98</v>
       </c>
       <c r="C27" s="12">
         <v>1966</v>
       </c>
       <c r="D27" s="10" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="E27" s="10" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="F27" s="10" t="s">
-        <v>92</v>
+        <v>99</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
       <c r="A28" s="10" t="s">
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="C28" s="12">
         <v>1967</v>
       </c>
       <c r="D28" s="10" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="E28" s="10" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="F28" s="10" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
       <c r="A29" s="10" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="C29" s="12">
         <v>1966</v>
       </c>
       <c r="D29" s="10" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="E29" s="10" t="s">
-        <v>57</v>
+        <v>95</v>
       </c>
       <c r="F29" s="10" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
       <c r="A30" s="10" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>99</v>
+        <v>106</v>
       </c>
       <c r="C30" s="12">
         <v>1965</v>
       </c>
       <c r="D30" s="10" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="E30" s="10" t="s">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="F30" s="10" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
       <c r="A31" s="10" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="C31" s="12">
         <v>1967</v>
       </c>
       <c r="D31" s="10" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="E31" s="10" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="F31" s="10" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75">
       <c r="A32" s="10" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="C32" s="12">
         <v>1967</v>
       </c>
       <c r="D32" s="10" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="E32" s="10" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="F32" s="10" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75">
       <c r="A33" s="10" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="C33" s="12">
         <v>1968</v>
       </c>
       <c r="D33" s="10" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="E33" s="10" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F33" s="10" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75">
       <c r="A34" s="10" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="C34" s="12">
         <v>1968</v>
       </c>
       <c r="D34" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="E34" s="10"/>
+        <v>84</v>
+      </c>
+      <c r="E34" s="10" t="s">
+        <v>121</v>
+      </c>
       <c r="F34" s="10" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18.75">
       <c r="A35" s="10" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="C35" s="12">
         <v>1971</v>
       </c>
       <c r="D35" s="10" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="E35" s="10" t="s">
-        <v>112</v>
+        <v>125</v>
       </c>
       <c r="F35" s="10" t="s">
-        <v>119</v>
+        <v>126</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18.75">
       <c r="A36" s="10" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>121</v>
+        <v>128</v>
       </c>
       <c r="C36" s="12">
         <v>1972</v>
       </c>
       <c r="D36" s="10" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="E36" s="10" t="s">
-        <v>112</v>
+        <v>121</v>
       </c>
       <c r="F36" s="10" t="s">
-        <v>122</v>
+        <v>129</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="18.75">
       <c r="A37" s="10" t="s">
-        <v>123</v>
+        <v>130</v>
       </c>
       <c r="B37" s="10" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
       <c r="C37" s="12">
         <v>1974</v>
       </c>
       <c r="D37" s="10" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="E37" s="10" t="s">
-        <v>112</v>
+        <v>121</v>
       </c>
       <c r="F37" s="10" t="s">
-        <v>125</v>
+        <v>132</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="18.75">
       <c r="A38" s="10" t="s">
-        <v>126</v>
+        <v>133</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>127</v>
+        <v>134</v>
       </c>
       <c r="C38" s="12">
         <v>1973</v>
       </c>
       <c r="D38" s="10" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="E38" s="10" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="F38" s="10" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="18.75">
       <c r="A39" s="10" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="B39" s="10" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="C39" s="12">
         <v>1978</v>
       </c>
       <c r="D39" s="10" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="E39" s="10" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="F39" s="10" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="18.75">
       <c r="A40" s="10" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="B40" s="10" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="C40" s="12">
         <v>1977</v>
       </c>
       <c r="D40" s="10" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="E40" s="10" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="F40" s="10" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="18.75">
       <c r="A41" s="10" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="B41" s="10" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="C41" s="12">
         <v>1991</v>
       </c>
       <c r="D41" s="10" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="E41" s="10" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="F41" s="10" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="18.75">
       <c r="A42" s="10" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="B42" s="10" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="C42" s="12">
         <v>2005</v>
       </c>
       <c r="D42" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="E42" s="10"/>
+        <v>84</v>
+      </c>
+      <c r="E42" s="10" t="s">
+        <v>149</v>
+      </c>
       <c r="F42" s="10" t="s">
-        <v>143</v>
+        <v>150</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="18.75">
       <c r="A43" s="10" t="s">
-        <v>144</v>
+        <v>151</v>
       </c>
       <c r="B43" s="10" t="s">
-        <v>145</v>
+        <v>152</v>
       </c>
       <c r="C43" s="12">
         <v>2006</v>
       </c>
       <c r="D43" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="E43" s="10"/>
+        <v>84</v>
+      </c>
+      <c r="E43" s="10" t="s">
+        <v>153</v>
+      </c>
       <c r="F43" s="10" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="18.75">
       <c r="A44" s="10" t="s">
-        <v>147</v>
+        <v>155</v>
       </c>
       <c r="B44" s="10" t="s">
-        <v>148</v>
+        <v>156</v>
       </c>
       <c r="C44" s="12">
         <v>1952</v>
       </c>
       <c r="D44" s="10" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
       <c r="E44" s="10" t="s">
-        <v>150</v>
+        <v>158</v>
       </c>
       <c r="F44" s="10" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="18.75">
       <c r="A45" s="10" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="B45" s="10" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="C45" s="12">
         <v>1953</v>
       </c>
       <c r="D45" s="10" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
       <c r="E45" s="10" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
       <c r="F45" s="10" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="18.75">
       <c r="A46" s="10" t="s">
-        <v>156</v>
+        <v>164</v>
       </c>
       <c r="B46" s="10" t="s">
-        <v>157</v>
+        <v>165</v>
       </c>
       <c r="C46" s="12">
         <v>1955</v>
       </c>
       <c r="D46" s="10" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
       <c r="E46" s="10" t="s">
-        <v>158</v>
+        <v>166</v>
       </c>
       <c r="F46" s="10" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="18.75">
       <c r="A47" s="10" t="s">
-        <v>160</v>
+        <v>168</v>
       </c>
       <c r="B47" s="10" t="s">
-        <v>161</v>
+        <v>169</v>
       </c>
       <c r="C47" s="12">
         <v>1956</v>
       </c>
       <c r="D47" s="10" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
       <c r="E47" s="10" t="s">
-        <v>162</v>
+        <v>170</v>
       </c>
       <c r="F47" s="10" t="s">
-        <v>163</v>
+        <v>171</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="18.75">
       <c r="A48" s="10" t="s">
-        <v>164</v>
+        <v>172</v>
       </c>
       <c r="B48" s="10" t="s">
-        <v>165</v>
+        <v>173</v>
       </c>
       <c r="C48" s="12">
         <v>1958</v>
       </c>
       <c r="D48" s="10" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
       <c r="E48" s="10" t="s">
-        <v>166</v>
+        <v>174</v>
       </c>
       <c r="F48" s="10" t="s">
-        <v>167</v>
+        <v>175</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="18.75">
       <c r="A49" s="10" t="s">
-        <v>168</v>
+        <v>176</v>
       </c>
       <c r="B49" s="10" t="s">
-        <v>169</v>
+        <v>177</v>
       </c>
       <c r="C49" s="12">
         <v>1958</v>
       </c>
       <c r="D49" s="10" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
       <c r="E49" s="10" t="s">
-        <v>170</v>
+        <v>178</v>
       </c>
       <c r="F49" s="10" t="s">
-        <v>171</v>
+        <v>179</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="18.75">
       <c r="A50" s="10" t="s">
-        <v>172</v>
+        <v>180</v>
       </c>
       <c r="B50" s="10" t="s">
-        <v>173</v>
+        <v>181</v>
       </c>
       <c r="C50" s="12">
         <v>1960</v>
       </c>
       <c r="D50" s="10" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
       <c r="E50" s="10" t="s">
-        <v>174</v>
+        <v>182</v>
       </c>
       <c r="F50" s="10" t="s">
-        <v>175</v>
+        <v>183</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="18.75">
       <c r="A51" s="10" t="s">
-        <v>176</v>
+        <v>184</v>
       </c>
       <c r="B51" s="10" t="s">
-        <v>177</v>
+        <v>185</v>
       </c>
       <c r="C51" s="12">
         <v>1961</v>
       </c>
       <c r="D51" s="10" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
       <c r="E51" s="10" t="s">
-        <v>178</v>
+        <v>186</v>
       </c>
       <c r="F51" s="10" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="18.75">
       <c r="A52" s="10" t="s">
-        <v>180</v>
+        <v>188</v>
       </c>
       <c r="B52" s="10" t="s">
-        <v>181</v>
+        <v>189</v>
       </c>
       <c r="C52" s="12">
         <v>1960</v>
       </c>
       <c r="D52" s="10" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
       <c r="E52" s="10" t="s">
-        <v>182</v>
+        <v>190</v>
       </c>
       <c r="F52" s="10" t="s">
-        <v>183</v>
+        <v>191</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="18.75">
       <c r="A53" s="10" t="s">
-        <v>184</v>
+        <v>192</v>
       </c>
       <c r="B53" s="10" t="s">
-        <v>185</v>
+        <v>193</v>
       </c>
       <c r="C53" s="12">
         <v>1961</v>
       </c>
       <c r="D53" s="10" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
       <c r="E53" s="10" t="s">
-        <v>186</v>
+        <v>194</v>
       </c>
       <c r="F53" s="10" t="s">
-        <v>187</v>
+        <v>195</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="18.75">
       <c r="A54" s="10" t="s">
-        <v>188</v>
+        <v>196</v>
       </c>
       <c r="B54" s="10" t="s">
-        <v>189</v>
+        <v>197</v>
       </c>
       <c r="C54" s="12">
         <v>1961</v>
       </c>
       <c r="D54" s="10" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
       <c r="E54" s="10" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
       <c r="F54" s="10" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="18.75">
       <c r="A55" s="10" t="s">
-        <v>192</v>
+        <v>200</v>
       </c>
       <c r="B55" s="10" t="s">
-        <v>193</v>
+        <v>201</v>
       </c>
       <c r="C55" s="12">
         <v>1961</v>
       </c>
       <c r="D55" s="10" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
       <c r="E55" s="10" t="s">
-        <v>194</v>
+        <v>202</v>
       </c>
       <c r="F55" s="10" t="s">
-        <v>195</v>
+        <v>203</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="18.75">
       <c r="A56" s="10" t="s">
-        <v>196</v>
+        <v>204</v>
       </c>
       <c r="B56" s="10" t="s">
-        <v>197</v>
+        <v>205</v>
       </c>
       <c r="C56" s="12">
         <v>1962</v>
       </c>
       <c r="D56" s="10" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
       <c r="E56" s="10" t="s">
-        <v>198</v>
+        <v>206</v>
       </c>
       <c r="F56" s="10" t="s">
-        <v>199</v>
+        <v>207</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="18.75">
       <c r="A57" s="10" t="s">
-        <v>200</v>
+        <v>208</v>
       </c>
       <c r="B57" s="10" t="s">
-        <v>201</v>
+        <v>209</v>
       </c>
       <c r="C57" s="12">
         <v>1962</v>
       </c>
       <c r="D57" s="10" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
       <c r="E57" s="10" t="s">
-        <v>202</v>
+        <v>210</v>
       </c>
       <c r="F57" s="10" t="s">
-        <v>203</v>
+        <v>211</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="18.75">
       <c r="A58" s="10" t="s">
-        <v>204</v>
+        <v>212</v>
       </c>
       <c r="B58" s="10" t="s">
-        <v>205</v>
+        <v>213</v>
       </c>
       <c r="C58" s="12">
         <v>1963</v>
       </c>
       <c r="D58" s="10" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
       <c r="E58" s="10" t="s">
-        <v>206</v>
+        <v>214</v>
       </c>
       <c r="F58" s="10" t="s">
-        <v>207</v>
+        <v>215</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="18.75">
       <c r="A59" s="10" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="B59" s="10" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="C59" s="12">
         <v>1963</v>
       </c>
       <c r="D59" s="10" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
       <c r="E59" s="10" t="s">
-        <v>210</v>
+        <v>218</v>
       </c>
       <c r="F59" s="10" t="s">
-        <v>211</v>
+        <v>219</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="18.75">
       <c r="A60" s="10" t="s">
-        <v>212</v>
+        <v>220</v>
       </c>
       <c r="B60" s="10" t="s">
-        <v>213</v>
+        <v>221</v>
       </c>
       <c r="C60" s="12">
         <v>1963</v>
       </c>
       <c r="D60" s="10" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
       <c r="E60" s="10" t="s">
-        <v>214</v>
+        <v>222</v>
       </c>
       <c r="F60" s="10" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="18.75">
       <c r="A61" s="10" t="s">
-        <v>216</v>
+        <v>224</v>
       </c>
       <c r="B61" s="10" t="s">
-        <v>217</v>
+        <v>225</v>
       </c>
       <c r="C61" s="12">
-        <v>1965</v>
+        <v>1964</v>
       </c>
       <c r="D61" s="10" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
       <c r="E61" s="10" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="F61" s="10" t="s">
-        <v>219</v>
+        <v>227</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="18.75">
       <c r="A62" s="10" t="s">
-        <v>220</v>
+        <v>228</v>
       </c>
       <c r="B62" s="10" t="s">
-        <v>221</v>
+        <v>229</v>
       </c>
       <c r="C62" s="12">
-        <v>1968</v>
+        <v>1965</v>
       </c>
       <c r="D62" s="10" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
       <c r="E62" s="10" t="s">
-        <v>222</v>
+        <v>230</v>
       </c>
       <c r="F62" s="10" t="s">
-        <v>223</v>
+        <v>231</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="18.75">
       <c r="A63" s="10" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="B63" s="10" t="s">
-        <v>225</v>
+        <v>233</v>
       </c>
       <c r="C63" s="12">
-        <v>1969</v>
+        <v>1968</v>
       </c>
       <c r="D63" s="10" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
       <c r="E63" s="10" t="s">
-        <v>226</v>
+        <v>234</v>
       </c>
       <c r="F63" s="10" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="18.75">
       <c r="A64" s="10" t="s">
-        <v>228</v>
+        <v>236</v>
       </c>
       <c r="B64" s="10" t="s">
-        <v>229</v>
+        <v>237</v>
       </c>
       <c r="C64" s="12">
-        <v>1974</v>
+        <v>1969</v>
       </c>
       <c r="D64" s="10" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
       <c r="E64" s="10" t="s">
-        <v>230</v>
+        <v>238</v>
       </c>
       <c r="F64" s="10" t="s">
-        <v>231</v>
+        <v>239</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="18.75">
       <c r="A65" s="10" t="s">
-        <v>232</v>
+        <v>240</v>
       </c>
       <c r="B65" s="10" t="s">
-        <v>233</v>
+        <v>241</v>
       </c>
       <c r="C65" s="12">
-        <v>1985</v>
+        <v>1974</v>
       </c>
       <c r="D65" s="10" t="s">
-        <v>149</v>
-      </c>
-      <c r="E65" s="10"/>
+        <v>157</v>
+      </c>
+      <c r="E65" s="10" t="s">
+        <v>242</v>
+      </c>
       <c r="F65" s="10" t="s">
-        <v>234</v>
+        <v>243</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="18.75">
       <c r="A66" s="10" t="s">
-        <v>235</v>
+        <v>244</v>
       </c>
       <c r="B66" s="10" t="s">
-        <v>236</v>
+        <v>245</v>
       </c>
       <c r="C66" s="12">
+        <v>1985</v>
+      </c>
+      <c r="D66" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="E66" s="10" t="s">
+        <v>246</v>
+      </c>
+      <c r="F66" s="10" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="67" customHeight="1" ht="18.75">
+      <c r="A67" s="10" t="s">
+        <v>248</v>
+      </c>
+      <c r="B67" s="10" t="s">
+        <v>249</v>
+      </c>
+      <c r="C67" s="12">
         <v>1999</v>
       </c>
-      <c r="D66" s="10" t="s">
-        <v>149</v>
-      </c>
-      <c r="E66" s="10" t="s">
-        <v>237</v>
-      </c>
-      <c r="F66" s="10" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="67" customHeight="1" ht="18.75">
-      <c r="A67" s="10"/>
-      <c r="B67" s="10"/>
-      <c r="C67" s="12"/>
-      <c r="D67" s="10"/>
-      <c r="E67" s="10"/>
-      <c r="F67" s="10"/>
+      <c r="D67" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="E67" s="10" t="s">
+        <v>250</v>
+      </c>
+      <c r="F67" s="10" t="s">
+        <v>251</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="68" customHeight="1" ht="18.75">
       <c r="A68" s="10"/>

</xml_diff>